<commit_message>
changed the sentences of background.
</commit_message>
<xml_diff>
--- a/portfolio03/01/ToDoList_要件定義・基本設計書.xlsx
+++ b/portfolio03/01/ToDoList_要件定義・基本設計書.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Programming\portfolio\portfolio03\01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C260B6-ECD4-4BBB-BC11-5F394025CBC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D85B349-7E33-4C83-9623-272D778EE14A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="758" xr2:uid="{B05C7E66-E09C-40F0-8B2A-CC0F0D5A8C2E}"/>
   </bookViews>
@@ -67,8 +67,8 @@
     <definedName name="_xlnm.Print_Area" localSheetId="11">動的振る舞い_ToDo登録機能!$A$1:$J$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">動的振る舞い_ToDo表示機能!$A$1:$J$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="12">動的振る舞い_ToDo編集機能!$A$1:$J$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="10">動的振る舞い_ログイン・ログアウト機能!$A$1:$J$78</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="14">動的振る舞い_管理者ログイン・ログアウト機能!$A$1:$J$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="10">動的振る舞い_ログイン・ログアウト機能!$A$1:$J$79</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="14">動的振る舞い_管理者ログイン・ログアウト機能!$A$1:$J$64</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">目的・背景!$A$1:$J$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">要件定義!$A$1:$J$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">要件定義_ToDo全表示機能!$A$1:$J$39</definedName>
@@ -182,12 +182,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>　ToDoListの開発に至ったきっかけは、開発者の所属している企業の業務の進め方に疑問を感じたことである。
-　開発者の所属している企業では、自身のすべき業務の期限や重要度を把握せずに業務を行っている社員が数多く存在していた。また、組織の管理者においても、組織に所属する社員の業務内容を把握しておらず、マネジメントがうまく機能していないケースが見受けられた。また、組織開発においても、各組織が抱えている業務と人員配置（人数、力量の両面）が一致していないケースが散見された。
-　ToDoListを活用することで、社員は自身の抱えている業務の期限や重要度を把握し、効率的な業務遂行の実現に繋げることができる。また、組織の管理者においても、各社員の抱える業務を正確に把握することで適切なマネジメントを行うことができる。組織開発においても、各組織が抱える業務から人員配置を決定することができ、最大限の成果を上げるための組織の構築に繋げることができる。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>図4-1　ToDoListの要求図</t>
     <rPh sb="0" eb="1">
       <t>ズ</t>
@@ -1844,6 +1838,72 @@
   </si>
   <si>
     <t>ユーザ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　ToDoListの開発に至ったきっかけは、業務の進め方やマネジメント、組織開発はもっと定量的なデータに基づいて行われるべきだと考えたからである。
+　日本の多くの企業では、IT技術の導入が遅れているという課題を抱えている。自身が抱えている業務について期限や重要度を把握せずに、ただ漠然と業務を行っている社員が数多く存在している。組織の管理者においても、組織に所属する社員の業務内容を把握しておらず、マネジメントがうまく機能していないケースが見受けられる。また、組織開発においても、各組織が抱えている業務と人員配置（人数、力量の両面）が一致していないケースが散見される。
+　今回開発したToDoListを活用することで、社員は自身の抱えている業務の期限や重要度を把握し、効率的な業務遂行の実現に繋げることができる。また、組織の管理者においても、各社員の抱える業務を正確に把握することで適切なマネジメントを行うことができる。組織開発においても、各組織が抱える業務から人員配置を決定することができ、最大限の成果を上げるための組織の構築に繋げることができる。</t>
+    <rPh sb="22" eb="24">
+      <t>ギョウム</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ソシキ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カイハツ</t>
+    </rPh>
+    <rPh sb="44" eb="47">
+      <t>テイリョウテキ</t>
+    </rPh>
+    <rPh sb="52" eb="53">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>カンガ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>ニホン</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ギジュツ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ドウニュウ</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>オク</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>カダイ</t>
+    </rPh>
+    <rPh sb="105" eb="106">
+      <t>カカ</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>カカ</t>
+    </rPh>
+    <rPh sb="140" eb="142">
+      <t>バクゼン</t>
+    </rPh>
+    <rPh sb="286" eb="288">
+      <t>コンカイ</t>
+    </rPh>
+    <rPh sb="288" eb="290">
+      <t>カイハツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2155,6 +2215,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2164,20 +2227,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2477,13 +2537,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>197211</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>13605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>639535</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>4907</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2745,16 +2805,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>56028</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>168087</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>67236</xdr:rowOff>
+      <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
+      <xdr:colOff>481853</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>167291</xdr:rowOff>
+      <xdr:rowOff>156085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2783,7 +2843,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="56028" y="1714501"/>
+          <a:off x="515469" y="1703295"/>
           <a:ext cx="5782237" cy="4806525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2851,15 +2911,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44824</xdr:colOff>
+      <xdr:colOff>537883</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:rowOff>56028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>593912</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>23434</xdr:rowOff>
+      <xdr:rowOff>45845</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2888,7 +2948,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392206" y="739588"/>
+          <a:off x="885265" y="761999"/>
           <a:ext cx="5334000" cy="3519670"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2955,14 +3015,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>345906</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>491584</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>22414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
+      <xdr:colOff>504266</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>4420</xdr:rowOff>
     </xdr:to>
@@ -2993,7 +3053,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="345906" y="728385"/>
+          <a:off x="838966" y="728385"/>
           <a:ext cx="5481153" cy="6100417"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3116,13 +3176,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44824</xdr:colOff>
+      <xdr:colOff>493059</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>682570</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447246</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
@@ -3153,7 +3213,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392206" y="750794"/>
+          <a:off x="840441" y="750794"/>
           <a:ext cx="5422658" cy="5390030"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3221,15 +3281,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>44823</xdr:colOff>
+      <xdr:colOff>481853</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>67235</xdr:rowOff>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
+      <xdr:colOff>448236</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>129487</xdr:rowOff>
+      <xdr:rowOff>151899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3258,7 +3318,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392205" y="773206"/>
+          <a:off x="829235" y="795618"/>
           <a:ext cx="5434854" cy="4533399"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3326,13 +3386,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>33618</xdr:colOff>
+      <xdr:colOff>459442</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>672353</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>414618</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>206506</xdr:rowOff>
     </xdr:to>
@@ -3363,7 +3423,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="381000" y="750794"/>
+          <a:off x="806824" y="750794"/>
           <a:ext cx="5423647" cy="5338800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3431,15 +3491,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>33619</xdr:colOff>
+      <xdr:colOff>526678</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>44824</xdr:rowOff>
+      <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>660861</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>470361</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>201707</xdr:rowOff>
+      <xdr:rowOff>224119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3468,7 +3528,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="381001" y="750795"/>
+          <a:off x="874060" y="773207"/>
           <a:ext cx="5412154" cy="5334000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3536,13 +3596,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
+      <xdr:colOff>470648</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>672353</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>437030</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>219654</xdr:rowOff>
     </xdr:to>
@@ -3573,7 +3633,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="369794" y="739588"/>
+          <a:off x="818030" y="739588"/>
           <a:ext cx="5434853" cy="5833801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3641,13 +3701,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
+      <xdr:colOff>504265</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>22412</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>653612</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>451906</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
@@ -3678,7 +3738,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="369794" y="728383"/>
+          <a:off x="851647" y="728383"/>
           <a:ext cx="5416112" cy="6028764"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3746,13 +3806,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>86222</xdr:colOff>
+      <xdr:colOff>568075</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>134472</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>618055</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>416349</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>56030</xdr:rowOff>
     </xdr:to>
@@ -3783,7 +3843,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="433604" y="605119"/>
+          <a:off x="915457" y="605119"/>
           <a:ext cx="5316745" cy="6275293"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3851,13 +3911,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>112060</xdr:colOff>
+      <xdr:colOff>582707</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>67236</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>672353</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>13779</xdr:rowOff>
     </xdr:to>
@@ -3888,7 +3948,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="459442" y="773207"/>
+          <a:off x="930089" y="773207"/>
           <a:ext cx="5345205" cy="4182366"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3956,13 +4016,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>145677</xdr:colOff>
+      <xdr:colOff>672353</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>617609</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>460726</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -3993,7 +4053,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="493059" y="750794"/>
+          <a:off x="1019735" y="750794"/>
           <a:ext cx="5256844" cy="6779559"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4061,13 +4121,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>22412</xdr:colOff>
+      <xdr:colOff>481853</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>661147</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>437029</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>62557</xdr:rowOff>
     </xdr:to>
@@ -4098,7 +4158,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="369794" y="750795"/>
+          <a:off x="829235" y="750795"/>
           <a:ext cx="5423647" cy="5430174"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4647,13 +4707,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>45358</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>229054</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>139954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4995,7 +5055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7107ED0-BA52-4BCC-B676-35520D163A00}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -5464,17 +5524,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -5499,11 +5559,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA45EC5-23D3-44FE-9826-5DF7DFE1A231}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:J62"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5512,12 +5570,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5541,22 +5599,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
@@ -5568,35 +5626,35 @@
       <c r="I32" s="31"/>
       <c r="J32" s="31"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A62" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-      <c r="H62" s="31"/>
-      <c r="I62" s="31"/>
-      <c r="J62" s="31"/>
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A63" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="A32:J32"/>
-    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="A63:J63"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -5618,17 +5676,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -5666,17 +5724,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
@@ -5712,17 +5770,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -5747,7 +5805,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E94CC6E-BD07-4ED9-B40B-816800972854}">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
@@ -5758,22 +5816,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -5785,32 +5843,32 @@
       <c r="I28" s="31"/>
       <c r="J28" s="31"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-    </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B41" t="s">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B42" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B61" s="31" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B60" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="31"/>
+      <c r="J61" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B60:J60"/>
+    <mergeCell ref="B61:J61"/>
     <mergeCell ref="A28:J28"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
@@ -5835,17 +5893,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -5885,12 +5943,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5914,7 +5972,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -5928,7 +5986,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -5957,9 +6015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A03FD7-9670-4BFC-99DF-6DE530E41E9F}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I4"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5974,12 +6030,12 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -5990,33 +6046,33 @@
       <c r="I2" s="30"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="A4" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
       <c r="H5" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -6024,16 +6080,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
       <c r="H6" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -6041,16 +6097,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="32"/>
       <c r="G7" s="32"/>
       <c r="H7" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -6058,16 +6114,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="32"/>
       <c r="G8" s="32"/>
       <c r="H8" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -6075,16 +6131,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F9" s="32"/>
       <c r="G9" s="32"/>
       <c r="H9" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -6092,16 +6148,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F10" s="32"/>
       <c r="G10" s="32"/>
       <c r="H10" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -6109,16 +6165,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="32"/>
       <c r="H11" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -6126,16 +6182,16 @@
         <v>7</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -6143,16 +6199,16 @@
         <v>8</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -6160,16 +6216,16 @@
         <v>9</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -6177,16 +6233,16 @@
         <v>10</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -6194,16 +6250,16 @@
         <v>11</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.4">
@@ -6211,22 +6267,22 @@
         <v>12</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I17" s="13"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
@@ -6248,7 +6304,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -6261,6 +6317,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:G17"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B33:I33"/>
     <mergeCell ref="C5:D5"/>
@@ -6277,21 +6348,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E8:G8"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -6304,9 +6360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B172754-F764-48F5-8812-6CE08F230582}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6316,12 +6370,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -6345,36 +6399,36 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B5" s="39" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B5" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -6388,7 +6442,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A63" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" s="31"/>
       <c r="C63" s="31"/>
@@ -6571,9 +6625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DD8AE6-B1F5-4DAB-847E-9B09FAFB1844}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6583,25 +6635,25 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
@@ -6615,7 +6667,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -6644,9 +6696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B799DC-77D5-49A6-8A35-1649471880BF}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6656,21 +6706,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -6938,7 +6988,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -6952,7 +7002,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A67" s="31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -6981,9 +7031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2D09B0-98C9-4DEC-936F-56D73D7DDE15}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -6993,21 +7041,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -7275,7 +7323,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -7289,7 +7337,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
@@ -7318,9 +7366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0DE416-210A-45BB-B655-2454DE4FC06E}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -7330,21 +7376,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -7590,7 +7636,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -7604,7 +7650,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A60" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B60" s="31"/>
       <c r="C60" s="31"/>
@@ -7645,21 +7691,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -7905,7 +7951,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -7919,7 +7965,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A64" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -7948,9 +7994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEE5679-CD28-4A40-8565-57470CB518BE}">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -7960,21 +8004,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -8220,7 +8264,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -8234,7 +8278,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A64" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -8263,9 +8307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61888F0-18EB-42D6-B0E5-3F7EB0B626D6}">
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -8275,21 +8317,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -8535,7 +8577,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -8549,7 +8591,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A66" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B66" s="31"/>
       <c r="C66" s="31"/>
@@ -8578,9 +8620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBD8C44-87AF-4D42-9249-56EAB4171B6F}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -8590,21 +8630,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -8850,7 +8890,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -8864,7 +8904,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A67" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -8893,9 +8933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A399CE8F-6181-47CF-AF79-A43EE379885E}">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -8905,21 +8943,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -9165,7 +9203,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -9179,7 +9217,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A73" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
@@ -9208,9 +9246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44454BB4-64AA-4EEE-BB76-A2797893E5DC}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -9220,21 +9256,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -9458,7 +9494,7 @@
     </row>
     <row r="23" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
@@ -9483,7 +9519,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A59" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -9512,7 +9548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E906CDDD-76E6-40EC-B28A-2D656FA7406A}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -9527,7 +9565,7 @@
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -9605,7 +9643,7 @@
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="30" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
@@ -9755,7 +9793,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B25" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
@@ -9789,9 +9827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F28B13-F143-4E07-A0C5-9CC09D429573}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -9801,21 +9837,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -10051,7 +10087,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -10065,7 +10101,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A76" s="31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B76" s="31"/>
       <c r="C76" s="31"/>
@@ -10094,9 +10130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE08DC08-DCB4-43E6-9AD8-348624817321}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -10106,21 +10140,21 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="19"/>
@@ -10356,7 +10390,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -10370,7 +10404,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A65" s="31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
@@ -10415,7 +10449,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B2" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -10439,7 +10473,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -10453,7 +10487,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -10467,31 +10501,31 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="36" t="s">
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="36"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="C20" s="10">
         <v>1</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="32"/>
     </row>
@@ -10500,13 +10534,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" s="32"/>
     </row>
@@ -10515,13 +10549,13 @@
         <v>3</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I22" s="32"/>
     </row>
@@ -10529,14 +10563,14 @@
       <c r="C23" s="10">
         <v>4</v>
       </c>
-      <c r="D23" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
+      <c r="D23" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
       <c r="H23" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I23" s="32"/>
     </row>
@@ -10544,14 +10578,14 @@
       <c r="C24" s="10">
         <v>5</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
+      <c r="D24" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
       <c r="H24" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I24" s="32"/>
     </row>
@@ -10560,13 +10594,13 @@
         <v>6</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I25" s="32"/>
     </row>
@@ -10580,6 +10614,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="D21:G21"/>
@@ -10596,7 +10631,6 @@
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="D23:G23"/>
     <mergeCell ref="D24:G24"/>
-    <mergeCell ref="H24:I24"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.39370078740157483" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -10618,22 +10652,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -10658,17 +10692,17 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -10707,17 +10741,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="31"/>
       <c r="C37" s="31"/>
@@ -10766,17 +10800,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -10812,17 +10846,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="31"/>
       <c r="C39" s="31"/>
@@ -10860,22 +10894,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
@@ -10889,17 +10923,17 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>

</xml_diff>